<commit_message>
modification of plan test
</commit_message>
<xml_diff>
--- a/plantTest.xlsx
+++ b/plantTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lim David\Desktop\site\Projet Openclassoom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lim David\Desktop\site\Projet Openclassoom\Kanap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0468D073-E8B5-442A-8014-EE58480C76CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA88380-5A33-449A-A779-BABFD7EB6AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,15 +46,9 @@
     <t>OK / Description erreur</t>
   </si>
   <si>
-    <t>La page produite donne la description (de manière dynamique) du produit sélectionné en page d'accueil.</t>
-  </si>
-  <si>
     <t>Sélectionner un produit dans la page d'accueil pour arriver à la page produit où la description spécifique de celle-ci est affiché.</t>
   </si>
   <si>
-    <t>Affiche la description de produit choisie.</t>
-  </si>
-  <si>
     <t>Sur la page produit on peut sélectionner la couleur et le nombre de produits que l'on souhaite acheter</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>Aller à la page panier pour voir les informations d'achat de l'utilisateur</t>
   </si>
   <si>
-    <t>Dans le panier le résumé des différentes informations des produits que l'utilisateur à choisis est affiché.</t>
-  </si>
-  <si>
     <t>Sur la page panier la quantité du produit est modifiable (compris entre 1-100). Le produit peut être supprimé et change donc les informations fournies sur le prix et le nombre total de produit.</t>
   </si>
   <si>
@@ -128,6 +119,15 @@
   </si>
   <si>
     <t>Ok</t>
+  </si>
+  <si>
+    <t>La page produit donne la description (de manière dynamique) du produit sélectionné en page d'accueil.</t>
+  </si>
+  <si>
+    <t>Affiche la description du produit choisie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> À la page panier le résumé des différentes informations des produits que l'utilisateur à choisis est affiché.</t>
   </si>
 </sst>
 </file>
@@ -688,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="76.8" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -737,16 +737,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="14" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="89.4" customHeight="1" x14ac:dyDescent="0.5">
@@ -754,50 +754,50 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>19</v>
-      </c>
       <c r="E6" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="120" customHeight="1" x14ac:dyDescent="0.5">
@@ -805,67 +805,67 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="115.2" customHeight="1" x14ac:dyDescent="0.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="91.2" customHeight="1" x14ac:dyDescent="0.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="61.8" customHeight="1" x14ac:dyDescent="0.5">
@@ -873,89 +873,89 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="21.6" x14ac:dyDescent="0.5">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>

</xml_diff>